<commit_message>
updated excel and plots.py
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\האחסון שלי\אקדמיה\האוניברסיטה העברית\קורסים\שנה ג\סמסטר ב\מבוא לבינה מלאכותית\מטלות\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C70D17-1A38-45BE-906D-DFC837F85B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F8EDD-1CF3-466E-9404-0DB5B6C293B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B185ED0C-F898-4113-ACB5-157695C9DA0D}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{B185ED0C-F898-4113-ACB5-157695C9DA0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Astar" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="21">
   <si>
     <t>Data set</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Mini Math</t>
+  </si>
+  <si>
+    <t>Mini Physics</t>
+  </si>
+  <si>
+    <t>UCS</t>
   </si>
 </sst>
 </file>
@@ -485,16 +494,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC75BA4-E9C4-4F04-AA12-B23A0E27743F}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.796875" style="2"/>
     <col min="4" max="4" width="10.09765625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.796875" style="2"/>
@@ -764,122 +773,68 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>63</v>
-      </c>
-      <c r="E14" s="2">
-        <v>78.594999999999999</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D15" s="2">
-        <v>381</v>
-      </c>
-      <c r="E15" s="2">
-        <v>78.721999999999994</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D16" s="2">
-        <v>139</v>
-      </c>
-      <c r="E16" s="2">
-        <v>79.165999999999997</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.03</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D17" s="2">
-        <v>63</v>
-      </c>
-      <c r="E17" s="2">
-        <v>68.524000000000001</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D18" s="2">
-        <v>381</v>
-      </c>
-      <c r="E18" s="2">
-        <v>66.635000000000005</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D19" s="2">
-        <v>139</v>
-      </c>
-      <c r="E19" s="2">
-        <v>71.578999999999994</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,16 +842,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2">
-        <v>78.908000000000001</v>
+        <v>78.594999999999999</v>
       </c>
       <c r="F20" s="2">
         <v>0.01</v>
@@ -907,19 +862,19 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="2">
-        <v>94</v>
+        <v>381</v>
       </c>
       <c r="E21" s="2">
-        <v>78.965999999999994</v>
+        <v>78.721999999999994</v>
       </c>
       <c r="F21" s="2">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,19 +882,19 @@
         <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="2">
-        <v>65958</v>
+        <v>139</v>
       </c>
       <c r="E22" s="2">
-        <v>78.5</v>
+        <v>79.165999999999997</v>
       </c>
       <c r="F22" s="2">
-        <v>10</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,19 +902,19 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="E23" s="2">
-        <v>79.44</v>
+        <v>68.524000000000001</v>
       </c>
       <c r="F23" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,19 +922,19 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="2">
-        <v>2105</v>
+        <v>381</v>
       </c>
       <c r="E24" s="2">
-        <v>80.082999999999998</v>
+        <v>66.635000000000005</v>
       </c>
       <c r="F24" s="2">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,19 +942,19 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="2">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="E25" s="2">
-        <v>80.082999999999998</v>
+        <v>71.578999999999994</v>
       </c>
       <c r="F25" s="2">
-        <v>7.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,16 +962,16 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="2">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2">
-        <v>75.977999999999994</v>
+        <v>78.908000000000001</v>
       </c>
       <c r="F26" s="2">
         <v>0.01</v>
@@ -1027,19 +982,19 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="2">
-        <v>363</v>
+        <v>94</v>
       </c>
       <c r="E27" s="2">
-        <v>75.62</v>
+        <v>78.965999999999994</v>
       </c>
       <c r="F27" s="2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,118 +1002,403 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="2">
-        <v>105683</v>
+        <v>65958</v>
       </c>
       <c r="E28" s="2">
-        <v>76.590999999999994</v>
+        <v>78.5</v>
       </c>
       <c r="F28" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="D29" s="2">
+        <v>24</v>
       </c>
       <c r="E29" s="2">
-        <v>80.150000000000006</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>17</v>
+        <v>79.44</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2105</v>
       </c>
       <c r="E30" s="2">
-        <v>81.325000000000003</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>17</v>
+        <v>80.082999999999998</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.15</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="D31" s="2">
+        <v>72</v>
       </c>
       <c r="E31" s="2">
-        <v>80.233000000000004</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>17</v>
+        <v>80.082999999999998</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="D32" s="2">
+        <v>43</v>
       </c>
       <c r="E32" s="2">
-        <v>84.606999999999999</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>17</v>
+        <v>75.977999999999994</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.01</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="D33" s="2">
+        <v>363</v>
       </c>
       <c r="E33" s="2">
+        <v>75.62</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2">
+        <v>105683</v>
+      </c>
+      <c r="E34" s="2">
+        <v>76.590999999999994</v>
+      </c>
+      <c r="F34" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="2">
+        <v>80.150000000000006</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="2">
+        <v>81.325000000000003</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="2">
+        <v>80.233000000000004</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="2">
+        <v>84.606999999999999</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="2">
         <v>78.817999999999998</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1170,16 +1410,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8729A61D-97FE-4E17-BE5D-4AD4726A2D83}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="2" customWidth="1"/>
     <col min="3" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
@@ -1367,86 +1607,68 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>78.594999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D15" s="2">
-        <v>78.721999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D16" s="2">
-        <v>79.165999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D17" s="2">
-        <v>68.524000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D18" s="2">
-        <v>66.635000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D19" s="2">
-        <v>71.578999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,13 +1676,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="2">
-        <v>78.908000000000001</v>
+        <v>78.594999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,13 +1690,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="2">
-        <v>78.965999999999994</v>
+        <v>78.721999999999994</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,13 +1704,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="2">
-        <v>78.5</v>
+        <v>79.165999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,13 +1718,13 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="2">
-        <v>79.44</v>
+        <v>68.524000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,13 +1732,13 @@
         <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="2">
-        <v>80.082999999999998</v>
+        <v>66.635000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,13 +1746,13 @@
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="2">
-        <v>80.082999999999998</v>
+        <v>71.578999999999994</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,13 +1760,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="2">
-        <v>75.977999999999994</v>
+        <v>78.908000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,13 +1774,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="2">
-        <v>75.62</v>
+        <v>78.965999999999994</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,83 +1788,261 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="2">
-        <v>76.590999999999994</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2">
-        <v>80.150000000000006</v>
+        <v>79.44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D30" s="2">
-        <v>81.325000000000003</v>
+        <v>80.082999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2">
-        <v>80.233000000000004</v>
+        <v>80.082999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D32" s="2">
-        <v>84.606999999999999</v>
+        <v>75.977999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D33" s="2">
+        <v>75.62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2">
+        <v>76.590999999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="2">
+        <v>80.150000000000006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="2">
+        <v>81.325000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2">
+        <v>80.233000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="2">
+        <v>84.606999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="2">
         <v>78.817999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="2">
+        <v>86.566000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="2">
+        <v>78.126999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel and unordered plots
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\האחסון שלי\אקדמיה\האוניברסיטה העברית\קורסים\שנה ג\סמסטר ב\מבוא לבינה מלאכותית\מטלות\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291F8EDD-1CF3-466E-9404-0DB5B6C293B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2FF69C-F610-46CF-8EA9-F2DC9DD8B07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{B185ED0C-F898-4113-ACB5-157695C9DA0D}"/>
+    <workbookView xWindow="456" yWindow="864" windowWidth="21636" windowHeight="11256" xr2:uid="{B185ED0C-F898-4113-ACB5-157695C9DA0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Astar" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="21">
   <si>
     <t>Data set</t>
   </si>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC75BA4-E9C4-4F04-AA12-B23A0E27743F}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -781,6 +781,15 @@
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D14" s="2">
+        <v>10021</v>
+      </c>
+      <c r="E14" s="2">
+        <v>85.05</v>
+      </c>
+      <c r="F14" s="2">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -792,6 +801,15 @@
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D15" s="2">
+        <v>192605</v>
+      </c>
+      <c r="E15" s="2">
+        <v>80.23</v>
+      </c>
+      <c r="F15" s="2">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -803,6 +821,15 @@
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D16" s="2">
+        <v>3327</v>
+      </c>
+      <c r="E16" s="2">
+        <v>79.33</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -814,6 +841,15 @@
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D17" s="2">
+        <v>363</v>
+      </c>
+      <c r="E17" s="2">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -825,6 +861,15 @@
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D18" s="2">
+        <v>206</v>
+      </c>
+      <c r="E18" s="2">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -836,6 +881,15 @@
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1147,6 +1201,15 @@
       <c r="C35" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D35" s="2">
+        <v>64</v>
+      </c>
+      <c r="E35" s="2">
+        <v>75.56</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -1158,6 +1221,15 @@
       <c r="C36" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D36" s="2">
+        <v>10532</v>
+      </c>
+      <c r="E36" s="2">
+        <v>76.13</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1169,6 +1241,15 @@
       <c r="C37" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D37" s="2">
+        <v>163</v>
+      </c>
+      <c r="E37" s="2">
+        <v>74.180000000000007</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -1180,6 +1261,15 @@
       <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D38" s="2">
+        <v>921</v>
+      </c>
+      <c r="E38" s="2">
+        <v>70.31</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1191,6 +1281,15 @@
       <c r="C39" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D39" s="2">
+        <v>10466</v>
+      </c>
+      <c r="E39" s="2">
+        <v>75.41</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -1201,6 +1300,15 @@
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,6 +1321,15 @@
       <c r="C41" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D41" s="2">
+        <v>1260027</v>
+      </c>
+      <c r="E41" s="2">
+        <v>84.46</v>
+      </c>
+      <c r="F41" s="2">
+        <v>150</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -1224,6 +1341,15 @@
       <c r="C42" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D42" s="2">
+        <v>135912</v>
+      </c>
+      <c r="E42" s="2">
+        <v>84.46</v>
+      </c>
+      <c r="F42" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -1235,6 +1361,15 @@
       <c r="C43" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D43" s="2">
+        <v>21960</v>
+      </c>
+      <c r="E43" s="2">
+        <v>83.01</v>
+      </c>
+      <c r="F43" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -1246,6 +1381,15 @@
       <c r="C44" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D44" s="2">
+        <v>1700926</v>
+      </c>
+      <c r="E44" s="2">
+        <v>85.05</v>
+      </c>
+      <c r="F44" s="2">
+        <v>300</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -1257,6 +1401,15 @@
       <c r="C45" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D45" s="2">
+        <v>1134098</v>
+      </c>
+      <c r="E45" s="2">
+        <v>80.23</v>
+      </c>
+      <c r="F45" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -1268,6 +1421,15 @@
       <c r="C46" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D46" s="2">
+        <v>52509</v>
+      </c>
+      <c r="E46" s="2">
+        <v>79.33</v>
+      </c>
+      <c r="F46" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -1279,6 +1441,15 @@
       <c r="C47" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D47" s="2">
+        <v>957805</v>
+      </c>
+      <c r="E47" s="2">
+        <v>77.930000000000007</v>
+      </c>
+      <c r="F47" s="2">
+        <v>280</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
@@ -1290,6 +1461,15 @@
       <c r="C48" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D48" s="2">
+        <v>957805</v>
+      </c>
+      <c r="E48" s="2">
+        <v>77.930000000000007</v>
+      </c>
+      <c r="F48" s="2">
+        <v>120</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -1301,6 +1481,15 @@
       <c r="C49" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -1367,7 +1556,7 @@
         <v>16</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>17</v>
@@ -1376,7 +1565,7 @@
         <v>17</v>
       </c>
       <c r="E53" s="2">
-        <v>84.606999999999999</v>
+        <v>78.817999999999998</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>17</v>
@@ -1387,7 +1576,7 @@
         <v>16</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>17</v>
@@ -1396,15 +1585,56 @@
         <v>17</v>
       </c>
       <c r="E54" s="2">
-        <v>78.817999999999998</v>
+        <v>84.606999999999999</v>
       </c>
       <c r="F54" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="2">
+        <v>86.566000000000003</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="2">
+        <v>78.126999999999995</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1412,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8729A61D-97FE-4E17-BE5D-4AD4726A2D83}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView rightToLeft="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add graph search plots
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\האחסון שלי\אקדמיה\האוניברסיטה העברית\קורסים\שנה ג\סמסטר ב\מבוא לבינה מלאכותית\מטלות\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9D3F2E-C262-4F89-8A1F-1E0E5A41DD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6F9026-AE85-4FD6-A817-D33997A2B25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15720" xr2:uid="{B185ED0C-F898-4113-ACB5-157695C9DA0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="21">
   <si>
     <t>Data set</t>
   </si>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC75BA4-E9C4-4F04-AA12-B23A0E27743F}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1433,19 +1433,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="2">
+        <v>80.150000000000006</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>17</v>
@@ -1453,19 +1453,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="2">
+        <v>81.325000000000003</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>17</v>
@@ -1473,19 +1473,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="2">
+        <v>80.233000000000004</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>17</v>
@@ -1493,19 +1493,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="2">
+        <v>84.606999999999999</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>17</v>
@@ -1513,19 +1513,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="2">
+        <v>86.566000000000003</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>17</v>
@@ -1533,221 +1533,21 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="2">
+        <v>78.126999999999995</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="2">
-        <v>4000000</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="2">
-        <v>80.150000000000006</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="2">
-        <v>81.325000000000003</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58" s="2">
-        <v>80.233000000000004</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59" s="2">
-        <v>78.817999999999998</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="2">
-        <v>84.606999999999999</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E61" s="2">
-        <v>86.566000000000003</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="2">
-        <v>78.126999999999995</v>
-      </c>
-      <c r="F62" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>